<commit_message>
已修改        gen_struct_cshap.py 缺失         in/cfg_2.xlsx 缺失         in/cfg_3.xlsx 已修改        in/test.xlsx 缺失         in/~$cfg_2.xlsx 已修改        out/config.cs 已修改        out/test.json 已修改        tojson.py
</commit_message>
<xml_diff>
--- a/in/test.xlsx
+++ b/in/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="1190" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,50 +22,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>number n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[bool] b_list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[number] n_list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[string] s_list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{bool} b_dict</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{number} n_dict</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{string} s_dict</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;bool b, number n, string s&gt; t</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[&lt;bool b, number n, string s&gt;] t_list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;&lt;bool b, number n, string s&gt; t&gt; t_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"b"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -126,18 +90,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{&lt;bool b, number n, string s&gt;} t_dict</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>//</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[{number}] d_list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[{"key0": 1, "key1": 2}, {"key0": 1, "key1": 2}]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -186,15 +142,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>number id</t>
+    <t>float id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>float n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>str s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[float] n_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[str] s_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{float} n_dict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{str} s_dict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;bool b, float n, strs&gt; t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[&lt;bool b, float n, str s&gt;] t_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{float}] d_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{&lt;bool b, float n, str s&gt;} t_dict</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;&lt;bool b, float n, str s&gt; t&gt; t_type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -327,6 +327,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -361,6 +362,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -536,103 +538,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="27.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="33.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="53.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="27.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="33.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="53.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -643,43 +645,43 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="L5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="O5" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -690,43 +692,43 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="M6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -737,40 +739,40 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -781,12 +783,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -794,12 +796,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>